<commit_message>
change boundary period attribution
- add column for filtering based on year relative to SEI-Trase dates
- delete versions saving from 2008-2024, etc
- move boundary period before attribution
</commit_message>
<xml_diff>
--- a/input-data/Economic Indicator_United States CPI Index, NSA__10 Apr 2025.xlsx
+++ b/input-data/Economic Indicator_United States CPI Index, NSA__10 Apr 2025.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/ucbvlm0_ucl_ac_uk/Documents/Documents/research/2025 IFB-Oxford AGILE/analysis/input_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/ucbvlm0_ucl_ac_uk/Documents/Documents/programming/main-projects/amazon-footprint/input-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{3E77A9E7-300F-F141-9577-51556034F463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C12A774-EA5D-7E4C-85D7-CB8D83523075}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{3E77A9E7-300F-F141-9577-51556034F463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F00BB1BF-1050-C74F-9671-43F0DC1D6B83}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="16660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6472,8 +6472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C1351"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A192" zoomScale="107" workbookViewId="0">
+      <selection activeCell="C202" sqref="C202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11" x14ac:dyDescent="0.15"/>

</xml_diff>